<commit_message>
Updating information for the following files:     legislative/abc_info.docx     legislative/acc_info.docx     legislative/pec_info.docx     member_list.xlsx Added an LEC function
</commit_message>
<xml_diff>
--- a/files/member_list.xlsx
+++ b/files/member_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bmt81\Documents\Personal Projects\SGA-Discord-Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bmt81\Documents\Personal Projects\SGA-Discord-Bot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD57F1B5-E880-435A-AA46-87420DB20C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB05A58-3348-4805-B50F-4A62A1C00DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="executive_board" sheetId="1" r:id="rId1"/>
     <sheet name="executive_cabinet" sheetId="5" r:id="rId2"/>
     <sheet name="legislative" sheetId="2" r:id="rId3"/>
-    <sheet name="judicial" sheetId="3" r:id="rId4"/>
+    <sheet name="lec" sheetId="6" r:id="rId4"/>
+    <sheet name="judicial" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>Brandon Townes</t>
   </si>
@@ -186,13 +187,43 @@
   </si>
   <si>
     <t>Jonathan Gauthier</t>
+  </si>
+  <si>
+    <t>ACC Chair</t>
+  </si>
+  <si>
+    <t>Senate President</t>
+  </si>
+  <si>
+    <t>Pro-Tempore</t>
+  </si>
+  <si>
+    <t>PEC Chair</t>
+  </si>
+  <si>
+    <t>ABC Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior Representative </t>
+  </si>
+  <si>
+    <t>Hannah Friday</t>
+  </si>
+  <si>
+    <t>ABC Vice-Chair</t>
+  </si>
+  <si>
+    <t>ACC Vice-Chair</t>
+  </si>
+  <si>
+    <t>PEC Vice-Chair</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +238,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -254,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,10 +308,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -322,6 +371,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9BCC3230-3B9C-4CBF-B741-94D66A433D8E}" name="Table136" displayName="Table136" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{9BCC3230-3B9C-4CBF-B741-94D66A433D8E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{85A18D4D-A8B8-4600-AC27-F6A7ABCEAB08}" name="Position"/>
+    <tableColumn id="2" xr3:uid="{C2A4FC56-80CF-4CE8-A4D3-63645A580271}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8A4CECBB-C67D-473F-AC35-568694A8BD13}" name="Table14" displayName="Table14" ref="A1:B6" totalsRowShown="0">
   <autoFilter ref="A1:B6" xr:uid="{8A4CECBB-C67D-473F-AC35-568694A8BD13}"/>
   <tableColumns count="2">
@@ -674,10 +737,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -772,7 +835,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,18 +950,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
+      <c r="A15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +973,180 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C86D5D-AF92-4755-9213-613757EF2104}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6F6F1B-73CC-4897-9633-17A3B8A90ADB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>